<commit_message>
Making it work for GCC
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Stack allocation</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>(300,1000)</t>
+  </si>
+  <si>
+    <t>MSVC</t>
+  </si>
+  <si>
+    <t>GCC</t>
+  </si>
+  <si>
+    <t>1,000 iteration (10,000 for 100 objects)</t>
   </si>
 </sst>
 </file>
@@ -78,7 +87,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -127,7 +136,7 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -433,79 +442,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
-        <v>140400900</v>
-      </c>
-      <c r="C2" s="1">
-        <v>46800300</v>
-      </c>
-      <c r="D2" s="1">
-        <v>78000500</v>
-      </c>
-      <c r="E2" s="1">
-        <v>171601100</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>62400400</v>
+        <v>140400900</v>
       </c>
       <c r="C3" s="1">
-        <v>15600100</v>
+        <v>46800300</v>
       </c>
       <c r="D3" s="1">
-        <v>31200200</v>
+        <v>78000500</v>
       </c>
       <c r="E3" s="1">
-        <v>62400400</v>
+        <v>171601100</v>
       </c>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -514,19 +504,19 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>109200700</v>
+        <v>62400400</v>
       </c>
       <c r="C4" s="1">
-        <v>31200200</v>
+        <v>15600100</v>
       </c>
       <c r="D4" s="1">
-        <v>78000500</v>
+        <v>31200200</v>
       </c>
       <c r="E4" s="1">
-        <v>156001000</v>
+        <v>62400400</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -538,22 +528,24 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>124800800</v>
+        <v>109200700</v>
       </c>
       <c r="C5" s="1">
         <v>31200200</v>
       </c>
       <c r="D5" s="1">
-        <v>46800300</v>
+        <v>78000500</v>
       </c>
       <c r="E5" s="1">
-        <v>109200700</v>
+        <v>156001000</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -562,19 +554,19 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>234001500</v>
+        <v>124800800</v>
       </c>
       <c r="C6" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="D6" s="1">
         <v>46800300</v>
       </c>
-      <c r="D6" s="1">
-        <v>93600600</v>
-      </c>
       <c r="E6" s="1">
-        <v>234001500</v>
+        <v>109200700</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -586,19 +578,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>187201200</v>
+        <v>234001500</v>
       </c>
       <c r="C7" s="1">
         <v>46800300</v>
       </c>
       <c r="D7" s="1">
-        <v>62400400</v>
+        <v>93600600</v>
       </c>
       <c r="E7" s="1">
-        <v>156001000</v>
+        <v>234001500</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -610,19 +602,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>156001000</v>
+        <v>187201200</v>
       </c>
       <c r="C8" s="1">
-        <v>31200200</v>
+        <v>46800300</v>
       </c>
       <c r="D8" s="1">
         <v>62400400</v>
       </c>
       <c r="E8" s="1">
-        <v>171601100</v>
+        <v>156001000</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -634,19 +626,19 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
-        <v>218401400</v>
+        <v>156001000</v>
       </c>
       <c r="C9" s="1">
-        <v>46800300</v>
+        <v>31200200</v>
       </c>
       <c r="D9" s="1">
-        <v>93600600</v>
+        <v>62400400</v>
       </c>
       <c r="E9" s="1">
-        <v>202801300</v>
+        <v>171601100</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -658,19 +650,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>62400400</v>
+        <v>218401400</v>
       </c>
       <c r="C10" s="1">
-        <v>15600100</v>
+        <v>46800300</v>
       </c>
       <c r="D10" s="1">
-        <v>15600100</v>
+        <v>93600600</v>
       </c>
       <c r="E10" s="1">
-        <v>46800300</v>
+        <v>202801300</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -681,10 +673,21 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1">
+        <v>62400400</v>
+      </c>
+      <c r="C11" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D11" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="E11" s="1">
+        <v>46800300</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -694,82 +697,78 @@
       <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="1">
-        <v>249601600</v>
-      </c>
-      <c r="C13" s="1">
-        <v>62400400</v>
-      </c>
-      <c r="D13" s="1">
-        <v>140400900</v>
-      </c>
-      <c r="E13" s="1">
-        <v>296401900</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B14" s="1">
-        <v>93600600</v>
+        <v>249601600</v>
       </c>
       <c r="C14" s="1">
-        <v>31200200</v>
+        <v>62400400</v>
       </c>
       <c r="D14" s="1">
-        <v>31200200</v>
+        <v>140400900</v>
       </c>
       <c r="E14" s="1">
-        <v>78000500</v>
+        <v>296401900</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1">
-        <v>171601100</v>
+        <v>93600600</v>
       </c>
       <c r="C15" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="D15" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E15" s="1">
         <v>78000500</v>
-      </c>
-      <c r="D15" s="1">
-        <v>140400900</v>
-      </c>
-      <c r="E15" s="1">
-        <v>156001000</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" s="1">
         <v>171601100</v>
       </c>
       <c r="C16" s="1">
-        <v>31200200</v>
+        <v>78000500</v>
       </c>
       <c r="D16" s="1">
-        <v>78000500</v>
+        <v>140400900</v>
       </c>
       <c r="E16" s="1">
         <v>156001000</v>
@@ -777,91 +776,549 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1">
-        <v>312002000</v>
+        <v>171601100</v>
       </c>
       <c r="C17" s="1">
-        <v>46800300</v>
+        <v>31200200</v>
       </c>
       <c r="D17" s="1">
-        <v>109200700</v>
+        <v>78000500</v>
       </c>
       <c r="E17" s="1">
-        <v>265201700</v>
+        <v>156001000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>202801300</v>
+        <v>312002000</v>
       </c>
       <c r="C18" s="1">
         <v>46800300</v>
       </c>
       <c r="D18" s="1">
-        <v>78000500</v>
+        <v>109200700</v>
       </c>
       <c r="E18" s="1">
-        <v>202801300</v>
+        <v>265201700</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1">
-        <v>249601600</v>
+        <v>202801300</v>
       </c>
       <c r="C19" s="1">
-        <v>31200200</v>
+        <v>46800300</v>
       </c>
       <c r="D19" s="1">
         <v>78000500</v>
       </c>
       <c r="E19" s="1">
-        <v>187201200</v>
+        <v>202801300</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1">
-        <v>234001500</v>
+        <v>249601600</v>
       </c>
       <c r="C20" s="1">
-        <v>46800300</v>
+        <v>31200200</v>
       </c>
       <c r="D20" s="1">
-        <v>93600600</v>
+        <v>78000500</v>
       </c>
       <c r="E20" s="1">
-        <v>218401400</v>
+        <v>187201200</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>234001500</v>
+      </c>
+      <c r="C21" s="1">
+        <v>46800300</v>
+      </c>
+      <c r="D21" s="1">
+        <v>93600600</v>
+      </c>
+      <c r="E21" s="1">
+        <v>218401400</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B22" s="1">
         <v>93600600</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C22" s="1">
         <v>15600100</v>
       </c>
-      <c r="D21" s="1">
-        <v>31200200</v>
-      </c>
-      <c r="E21" s="1">
+      <c r="D22" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E22" s="1">
         <v>78000500</v>
       </c>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>109200700</v>
+      </c>
+      <c r="C27" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D27" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E27" s="1">
+        <v>78000500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <v>62400400</v>
+      </c>
+      <c r="C28" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D28" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E28" s="1">
+        <v>62400400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <v>124800800</v>
+      </c>
+      <c r="C29" s="1">
+        <v>46800300</v>
+      </c>
+      <c r="D29" s="1">
+        <v>78000500</v>
+      </c>
+      <c r="E29" s="1">
+        <v>187201200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>124800800</v>
+      </c>
+      <c r="C30" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="D30" s="1">
+        <v>46800300</v>
+      </c>
+      <c r="E30" s="1">
+        <v>109200700</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1029606600</v>
+      </c>
+      <c r="C31" s="1">
+        <v>202801300</v>
+      </c>
+      <c r="D31" s="1">
+        <v>436802800</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1123207200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="1">
+        <v>998406400</v>
+      </c>
+      <c r="C32" s="1">
+        <v>202801300</v>
+      </c>
+      <c r="D32" s="1">
+        <v>421202700</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1076406900</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="1">
+        <v>218401400</v>
+      </c>
+      <c r="C33" s="1">
+        <v>46800300</v>
+      </c>
+      <c r="D33" s="1">
+        <v>78000500</v>
+      </c>
+      <c r="E33" s="1">
+        <v>202801300</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="1">
+        <v>982806300</v>
+      </c>
+      <c r="C34" s="1">
+        <v>202801300</v>
+      </c>
+      <c r="D34" s="1">
+        <v>421202700</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1092007000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="1">
+        <v>62400400</v>
+      </c>
+      <c r="C35" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D35" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="E35" s="1">
+        <v>31200200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="1">
+        <v>202801300</v>
+      </c>
+      <c r="C38" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="D38" s="1">
+        <v>62400400</v>
+      </c>
+      <c r="E38" s="1">
+        <v>218401400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="1">
+        <v>124800800</v>
+      </c>
+      <c r="C39" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D39" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E39" s="1">
+        <v>93600600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="1">
+        <v>296401900</v>
+      </c>
+      <c r="C40" s="1">
+        <v>78000500</v>
+      </c>
+      <c r="D40" s="1">
+        <v>124800800</v>
+      </c>
+      <c r="E40" s="1">
+        <v>218401400</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="1">
+        <v>234001500</v>
+      </c>
+      <c r="C41" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="D41" s="1">
+        <v>62400400</v>
+      </c>
+      <c r="E41" s="1">
+        <v>156001000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1232407900</v>
+      </c>
+      <c r="C42" s="1">
+        <v>202801300</v>
+      </c>
+      <c r="D42" s="1">
+        <v>452402900</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1154407400</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1060806800</v>
+      </c>
+      <c r="C43" s="1">
+        <v>218401400</v>
+      </c>
+      <c r="D43" s="1">
+        <v>452402900</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1138807300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="1">
+        <v>280801800</v>
+      </c>
+      <c r="C44" s="1">
+        <v>46800300</v>
+      </c>
+      <c r="D44" s="1">
+        <v>109200700</v>
+      </c>
+      <c r="E44" s="1">
+        <v>218401400</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1045206700</v>
+      </c>
+      <c r="C45" s="1">
+        <v>218401400</v>
+      </c>
+      <c r="D45" s="1">
+        <v>421202700</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1123207200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>78000500</v>
+      </c>
+      <c r="C46" s="1">
+        <v>15600100</v>
+      </c>
+      <c r="D46" s="1">
+        <v>31200200</v>
+      </c>
+      <c r="E46" s="1">
+        <v>62400400</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B10">
+  <conditionalFormatting sqref="B3:B11">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C11">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D11">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E11">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:B22">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C22">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:D22">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14:E22">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:B35">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -873,7 +1330,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C10">
+  <conditionalFormatting sqref="C27:C35">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -885,7 +1342,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D10">
+  <conditionalFormatting sqref="D27:D35">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -897,7 +1354,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E10">
+  <conditionalFormatting sqref="E27:E35">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -909,7 +1366,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B21">
+  <conditionalFormatting sqref="B38:B46">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -921,7 +1378,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13:C21">
+  <conditionalFormatting sqref="C38:C46">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -933,7 +1390,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D21">
+  <conditionalFormatting sqref="D38:D46">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -945,7 +1402,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13:E21">
+  <conditionalFormatting sqref="E38:E46">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>